<commit_message>
fix： tons of problems
</commit_message>
<xml_diff>
--- a/asserts/coords_tracking/VERDANTURF TOWN coordinates.xlsx
+++ b/asserts/coords_tracking/VERDANTURF TOWN coordinates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SS\Documents\GitHub\pokemmo_py_auto\asserts\coords_tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7DC11A4-8A2B-414C-86F7-864F5682D611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7D05E5-9BBA-4E3B-9315-585F7F4CD03A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="2">
   <si>
     <t>pc_in</t>
   </si>
@@ -393,8 +393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="AQ25" sqref="AQ25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AO7" sqref="AO7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.7109375" defaultRowHeight="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -522,22 +522,22 @@
       <c r="A2" s="1">
         <v>-15</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2">
         <v>1</v>
       </c>
     </row>
@@ -545,25 +545,25 @@
       <c r="A3" s="1">
         <v>-14</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC3" s="2" t="s">
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC3" s="2">
         <v>1</v>
       </c>
     </row>
@@ -571,16 +571,16 @@
       <c r="A4" s="1">
         <v>-13</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC4" s="2" t="s">
+      <c r="G4" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC4" s="2">
         <v>1</v>
       </c>
     </row>
@@ -588,13 +588,13 @@
       <c r="A5" s="1">
         <v>-12</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2">
         <v>1</v>
       </c>
       <c r="F5" s="2" t="s">
@@ -657,13 +657,13 @@
       <c r="Y5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Z5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB5" s="2" t="s">
+      <c r="Z5" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="2">
         <v>1</v>
       </c>
     </row>
@@ -671,13 +671,13 @@
       <c r="A6" s="1">
         <v>-11</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2">
         <v>1</v>
       </c>
       <c r="F6" s="2" t="s">
@@ -740,16 +740,16 @@
       <c r="Y6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="Z6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC6" s="2" t="s">
+      <c r="Z6" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC6" s="2">
         <v>1</v>
       </c>
     </row>
@@ -757,19 +757,19 @@
       <c r="A7" s="1">
         <v>-10</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD7" s="2" t="s">
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC7" s="2">
+        <v>1</v>
+      </c>
+      <c r="AD7" s="2">
         <v>1</v>
       </c>
     </row>
@@ -792,19 +792,19 @@
       <c r="F8" s="2">
         <v>1</v>
       </c>
-      <c r="AA8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE8" s="2" t="s">
+      <c r="AA8" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB8" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC8" s="2">
+        <v>1</v>
+      </c>
+      <c r="AD8" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE8" s="2">
         <v>1</v>
       </c>
     </row>
@@ -827,22 +827,22 @@
       <c r="F9" s="2">
         <v>1</v>
       </c>
-      <c r="AA9" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB9" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC9" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD9" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE9" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF9" s="2" t="s">
+      <c r="AA9" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB9" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC9" s="2">
+        <v>1</v>
+      </c>
+      <c r="AD9" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE9" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF9" s="2">
         <v>1</v>
       </c>
     </row>
@@ -865,22 +865,22 @@
       <c r="F10" s="2">
         <v>1</v>
       </c>
-      <c r="AA10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AF10" s="2" t="s">
+      <c r="AA10" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB10" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC10" s="2">
+        <v>1</v>
+      </c>
+      <c r="AD10" s="2">
+        <v>1</v>
+      </c>
+      <c r="AE10" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF10" s="2">
         <v>1</v>
       </c>
     </row>
@@ -900,7 +900,7 @@
       <c r="E11" s="2">
         <v>1</v>
       </c>
-      <c r="AB11" s="2" t="s">
+      <c r="AB11" s="2">
         <v>1</v>
       </c>
     </row>
@@ -908,10 +908,10 @@
       <c r="A12" s="1">
         <v>-5</v>
       </c>
-      <c r="AB12" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC12" s="2" t="s">
+      <c r="AB12" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC12" s="2">
         <v>1</v>
       </c>
     </row>
@@ -919,13 +919,13 @@
       <c r="A13" s="1">
         <v>-4</v>
       </c>
-      <c r="AB13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD13" s="2" t="s">
+      <c r="AB13" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC13" s="2">
+        <v>1</v>
+      </c>
+      <c r="AD13" s="2">
         <v>1</v>
       </c>
     </row>
@@ -942,19 +942,19 @@
       <c r="X14" s="2">
         <v>1</v>
       </c>
-      <c r="Z14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AD14" s="2" t="s">
+      <c r="Z14" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA14" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB14" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC14" s="2">
+        <v>1</v>
+      </c>
+      <c r="AD14" s="2">
         <v>1</v>
       </c>
     </row>
@@ -1244,9 +1244,6 @@
     <row r="23" spans="1:39" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>6</v>
-      </c>
-      <c r="T23" s="2">
-        <v>1</v>
       </c>
       <c r="Z23" s="2">
         <v>1</v>

</xml_diff>